<commit_message>
update result data, using high resolution timer
</commit_message>
<xml_diff>
--- a/reports/benchmark_result.xlsx
+++ b/reports/benchmark_result.xlsx
@@ -6445,11 +6445,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="49429504"/>
-        <c:axId val="49427968"/>
+        <c:axId val="132072192"/>
+        <c:axId val="132073728"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="49429504"/>
+        <c:axId val="132072192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6459,12 +6459,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49427968"/>
+        <c:crossAx val="132073728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="49427968"/>
+        <c:axId val="132073728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6501,14 +6501,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="49429504"/>
+        <c:crossAx val="132072192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -6868,9 +6867,6 @@
                 <c:pt idx="98">
                   <c:v>990000</c:v>
                 </c:pt>
-                <c:pt idx="99">
-                  <c:v>1000000</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6881,304 +6877,301 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.01</c:v>
+                  <c:v>1.2999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.01</c:v>
+                  <c:v>1.2E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.01</c:v>
+                  <c:v>1.2999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.01</c:v>
+                  <c:v>1.7999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.02</c:v>
+                  <c:v>2.5999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.02</c:v>
+                  <c:v>2.5999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.02</c:v>
+                  <c:v>3.1E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.02</c:v>
+                  <c:v>2.8000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.03</c:v>
+                  <c:v>4.7E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.03</c:v>
+                  <c:v>4.5999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.04</c:v>
+                  <c:v>7.3999999999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.04</c:v>
+                  <c:v>6.9000000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.04</c:v>
+                  <c:v>5.8999999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.05</c:v>
+                  <c:v>5.8999999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.05</c:v>
+                  <c:v>6.2E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.05</c:v>
+                  <c:v>6.6000000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.06</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.06</c:v>
+                  <c:v>6.6000000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.06</c:v>
+                  <c:v>7.5999999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.06</c:v>
+                  <c:v>7.8E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.06</c:v>
+                  <c:v>8.5000000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>9.1999999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.09</c:v>
+                  <c:v>9.9000000000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.1</c:v>
+                  <c:v>0.128</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.1</c:v>
+                  <c:v>0.124</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.11</c:v>
+                  <c:v>0.126</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.1</c:v>
+                  <c:v>0.122</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.11</c:v>
+                  <c:v>0.127</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.11</c:v>
+                  <c:v>0.127</c:v>
                 </c:pt>
                 <c:pt idx="31">
+                  <c:v>0.14299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.14699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.14299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.154</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.16300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.154</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.16400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.155</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.16900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.17100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="42">
                   <c:v>0.18</c:v>
                 </c:pt>
-                <c:pt idx="32">
-                  <c:v>0.11</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>0.13</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>0.13</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>0.12</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>0.13</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>0.13</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>0.13</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>0.14000000000000001</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.14000000000000001</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>0.15</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>0.15</c:v>
-                </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.16</c:v>
+                  <c:v>0.17599999999999999</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.16</c:v>
+                  <c:v>0.17799999999999999</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.15</c:v>
+                  <c:v>0.184</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.17</c:v>
+                  <c:v>0.182</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.17</c:v>
+                  <c:v>0.19</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.18</c:v>
+                  <c:v>0.186</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.18</c:v>
+                  <c:v>0.191</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.17</c:v>
+                  <c:v>0.19500000000000001</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.18</c:v>
+                  <c:v>0.20300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.24</c:v>
+                  <c:v>0.25900000000000001</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.26</c:v>
+                  <c:v>0.27500000000000002</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.25</c:v>
+                  <c:v>0.27600000000000002</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.27</c:v>
+                  <c:v>0.28100000000000003</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.27</c:v>
+                  <c:v>0.28799999999999998</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.27</c:v>
+                  <c:v>0.27800000000000002</c:v>
                 </c:pt>
                 <c:pt idx="58">
                   <c:v>0.28999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.28999999999999998</c:v>
+                  <c:v>0.32200000000000001</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.28999999999999998</c:v>
+                  <c:v>0.30399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.26</c:v>
+                  <c:v>0.29599999999999999</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.27</c:v>
+                  <c:v>0.29899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.28999999999999998</c:v>
+                  <c:v>0.316</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.31</c:v>
+                  <c:v>0.30299999999999999</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.28000000000000003</c:v>
+                  <c:v>0.30599999999999999</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.32</c:v>
+                  <c:v>0.311</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.28999999999999998</c:v>
+                  <c:v>0.33100000000000002</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.31</c:v>
+                  <c:v>0.317</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.3</c:v>
+                  <c:v>0.31900000000000001</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.31</c:v>
+                  <c:v>0.318</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.31</c:v>
+                  <c:v>0.32900000000000001</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.33</c:v>
+                  <c:v>0.34300000000000003</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.32</c:v>
+                  <c:v>0.33600000000000002</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.31</c:v>
+                  <c:v>0.34200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="75">
+                  <c:v>0.35399999999999998</c:v>
+                </c:pt>
+                <c:pt idx="76">
                   <c:v>0.35</c:v>
                 </c:pt>
-                <c:pt idx="76">
-                  <c:v>0.34</c:v>
-                </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.35</c:v>
+                  <c:v>0.36</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.34</c:v>
+                  <c:v>0.34499999999999997</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.33</c:v>
+                  <c:v>0.34699999999999998</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.36</c:v>
+                  <c:v>0.36599999999999999</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.35</c:v>
+                  <c:v>0.36399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.36</c:v>
+                  <c:v>0.36399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.34</c:v>
+                  <c:v>0.36399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.36</c:v>
+                  <c:v>0.36899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.37</c:v>
+                  <c:v>0.38800000000000001</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.4</c:v>
+                  <c:v>0.38500000000000001</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.37</c:v>
+                  <c:v>0.38200000000000001</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.39</c:v>
+                  <c:v>0.378</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.38</c:v>
+                  <c:v>0.38700000000000001</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.41</c:v>
+                  <c:v>0.40200000000000002</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.38</c:v>
+                  <c:v>0.39500000000000002</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.38</c:v>
+                  <c:v>0.39600000000000002</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.41</c:v>
+                  <c:v>0.39500000000000002</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.39</c:v>
+                  <c:v>0.42</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.4</c:v>
+                  <c:v>0.41699999999999998</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.41</c:v>
+                  <c:v>0.41499999999999998</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.4</c:v>
+                  <c:v>0.42199999999999999</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.39</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>0.39</c:v>
+                  <c:v>0.42799999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7510,9 +7503,6 @@
                 <c:pt idx="98">
                   <c:v>990000</c:v>
                 </c:pt>
-                <c:pt idx="99">
-                  <c:v>1000000</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -7523,43 +7513,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.01</c:v>
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.01</c:v>
+                  <c:v>8.0000000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>8.0000000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.01</c:v>
+                  <c:v>5.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>8.0000000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.01</c:v>
+                  <c:v>1.0999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.01</c:v>
+                  <c:v>8.0000000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>1.0999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.01</c:v>
+                  <c:v>1.2E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.01</c:v>
+                  <c:v>8.9999999999999993E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.01</c:v>
@@ -7568,82 +7558,82 @@
                   <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.01</c:v>
+                  <c:v>1.2999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.02</c:v>
+                  <c:v>1.2E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.01</c:v>
+                  <c:v>1.2999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.01</c:v>
+                  <c:v>1.4999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.01</c:v>
+                  <c:v>1.7000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.02</c:v>
+                  <c:v>1.9E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.02</c:v>
+                  <c:v>2.7E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.02</c:v>
+                  <c:v>2.1999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.02</c:v>
+                  <c:v>2.1999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.02</c:v>
+                  <c:v>2.5000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.02</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.03</c:v>
+                  <c:v>2.5999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.03</c:v>
+                  <c:v>3.2000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.03</c:v>
+                  <c:v>3.1E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.03</c:v>
+                  <c:v>3.1E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.03</c:v>
+                  <c:v>2.9000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.06</c:v>
+                  <c:v>3.5000000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.04</c:v>
+                  <c:v>3.9E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.04</c:v>
+                  <c:v>3.5000000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.03</c:v>
+                  <c:v>3.6999999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.04</c:v>
+                  <c:v>4.3999999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.04</c:v>
+                  <c:v>4.1000000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.04</c:v>
+                  <c:v>4.4999999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
+                  <c:v>4.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
                   <c:v>0.05</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>0.05</c:v>
@@ -7655,172 +7645,169 @@
                   <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.05</c:v>
+                  <c:v>5.7000000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.06</c:v>
+                  <c:v>6.5000000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.05</c:v>
+                  <c:v>6.0999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.06</c:v>
+                  <c:v>5.8000000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.06</c:v>
+                  <c:v>6.4000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.06</c:v>
+                  <c:v>6.7000000000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>7.4999999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.06</c:v>
+                  <c:v>7.0999999999999994E-2</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>6.8000000000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>6.9000000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.06</c:v>
+                  <c:v>6.7000000000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>7.0999999999999994E-2</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>8.1000000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.08</c:v>
+                  <c:v>7.6999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>7.3999999999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.08</c:v>
+                  <c:v>7.6999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="61">
                   <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.08</c:v>
+                  <c:v>8.7999999999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.08</c:v>
+                  <c:v>8.3000000000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.08</c:v>
+                  <c:v>8.5000000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="65">
+                  <c:v>9.4E-2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>8.7999999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="67">
                   <c:v>0.09</c:v>
                 </c:pt>
-                <c:pt idx="66">
-                  <c:v>0.08</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>0.1</c:v>
-                </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.1</c:v>
+                  <c:v>9.2999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.09</c:v>
+                  <c:v>9.4E-2</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.1</c:v>
+                  <c:v>9.9000000000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.09</c:v>
+                  <c:v>0.104</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.11</c:v>
+                  <c:v>9.9000000000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.11</c:v>
+                  <c:v>9.9000000000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.1</c:v>
+                  <c:v>0.10199999999999999</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.12</c:v>
+                  <c:v>0.106</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.12</c:v>
+                  <c:v>0.11799999999999999</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.12</c:v>
+                  <c:v>0.107</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.11</c:v>
+                  <c:v>0.108</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.11</c:v>
+                  <c:v>0.111</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.12</c:v>
+                  <c:v>0.115</c:v>
                 </c:pt>
                 <c:pt idx="81">
+                  <c:v>0.124</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.11799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.11899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.13100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.121</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.13400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.128</c:v>
+                </c:pt>
+                <c:pt idx="88">
                   <c:v>0.13</c:v>
                 </c:pt>
-                <c:pt idx="82">
-                  <c:v>0.13</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>0.12</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>0.12</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>0.12</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>0.14000000000000001</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>0.14000000000000001</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>0.15</c:v>
-                </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.14000000000000001</c:v>
+                  <c:v>0.14499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.15</c:v>
+                  <c:v>0.13800000000000001</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.14000000000000001</c:v>
+                  <c:v>0.13500000000000001</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.15</c:v>
+                  <c:v>0.14099999999999999</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.16</c:v>
+                  <c:v>0.14299999999999999</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.16</c:v>
+                  <c:v>0.14299999999999999</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.14000000000000001</c:v>
+                  <c:v>0.14399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.16</c:v>
+                  <c:v>0.14399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.16</c:v>
+                  <c:v>0.153</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.15</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>0.16</c:v>
+                  <c:v>0.156</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8150,9 +8137,6 @@
                 <c:pt idx="98">
                   <c:v>990000</c:v>
                 </c:pt>
-                <c:pt idx="99">
-                  <c:v>1000000</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -8163,304 +8147,301 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
                 <c:pt idx="0">
-                  <c:v>0.01</c:v>
+                  <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.01</c:v>
+                  <c:v>6.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>5.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.01</c:v>
+                  <c:v>8.9999999999999993E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.01</c:v>
+                  <c:v>8.9999999999999993E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.6E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.7000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.9E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>0.02</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.01</c:v>
-                </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.02</c:v>
+                  <c:v>2.1000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v>3.1E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.2000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.2000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.3000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.5999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.5000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.6999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.7999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.9E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>0.04</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.03</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.04</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.03</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.03</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.04</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.04</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.04</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.04</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.04</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.03</c:v>
-                </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.04</c:v>
+                  <c:v>4.2000000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.05</c:v>
+                  <c:v>4.2999999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.06</c:v>
+                  <c:v>6.5000000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.06</c:v>
+                  <c:v>6.2E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>6.3E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.06</c:v>
+                  <c:v>7.0999999999999994E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>6.5000000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>6.9000000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.06</c:v>
+                  <c:v>7.0999999999999994E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.06</c:v>
+                  <c:v>7.0999999999999994E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>6.9000000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.08</c:v>
+                  <c:v>8.2000000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.08</c:v>
+                  <c:v>7.3999999999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.08</c:v>
+                  <c:v>7.6999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.08</c:v>
+                  <c:v>7.9000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.08</c:v>
+                  <c:v>8.1000000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>8.2000000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="41">
                   <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="42">
+                  <c:v>8.3000000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
                   <c:v>0.08</c:v>
                 </c:pt>
-                <c:pt idx="43">
-                  <c:v>7.0000000000000007E-2</c:v>
-                </c:pt>
                 <c:pt idx="44">
+                  <c:v>8.3000000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>9.0999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
                   <c:v>0.09</c:v>
                 </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.08</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0.1</c:v>
-                </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.09</c:v>
+                  <c:v>8.5000000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.08</c:v>
+                  <c:v>8.7999999999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.1</c:v>
+                  <c:v>9.1999999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.09</c:v>
+                  <c:v>0.10299999999999999</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.1</c:v>
+                  <c:v>9.7000000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.15</c:v>
+                  <c:v>0.13600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.14000000000000001</c:v>
+                  <c:v>0.13900000000000001</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>0.14000000000000001</c:v>
+                  <c:v>0.14199999999999999</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>0.15</c:v>
+                  <c:v>0.14299999999999999</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.15</c:v>
+                  <c:v>0.14299999999999999</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.15</c:v>
+                  <c:v>0.14699999999999999</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.15</c:v>
+                  <c:v>0.14299999999999999</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.16</c:v>
+                  <c:v>0.153</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.16</c:v>
+                  <c:v>0.158</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.15</c:v>
+                  <c:v>0.152</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.16</c:v>
+                  <c:v>0.14699999999999999</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.15</c:v>
+                  <c:v>0.156</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.15</c:v>
+                  <c:v>0.16800000000000001</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.16</c:v>
+                  <c:v>0.153</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.15</c:v>
+                  <c:v>0.16200000000000001</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.16</c:v>
+                  <c:v>0.16300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.17</c:v>
+                  <c:v>0.161</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.16</c:v>
+                  <c:v>0.182</c:v>
                 </c:pt>
                 <c:pt idx="70">
+                  <c:v>0.16600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.17199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.16900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.17399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.17699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.17899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.19600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="78">
                   <c:v>0.19</c:v>
                 </c:pt>
-                <c:pt idx="71">
-                  <c:v>0.17</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>0.19</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>0.17</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>0.17</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>0.19</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>0.2</c:v>
-                </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.19</c:v>
+                  <c:v>0.185</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.18</c:v>
+                  <c:v>0.17599999999999999</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.18</c:v>
+                  <c:v>0.189</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.19</c:v>
+                  <c:v>0.193</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.19</c:v>
+                  <c:v>0.20100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>0.19</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.19</c:v>
+                  <c:v>0.191</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.23</c:v>
+                  <c:v>0.20300000000000001</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.2</c:v>
+                  <c:v>0.19800000000000001</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.19</c:v>
+                  <c:v>0.20100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.2</c:v>
+                  <c:v>0.217</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>0.24</c:v>
+                  <c:v>0.21</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>0.23</c:v>
+                  <c:v>0.20899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>0.25</c:v>
+                  <c:v>0.20399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>0.23</c:v>
+                  <c:v>0.20899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>0.2</c:v>
+                  <c:v>0.215</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>0.23</c:v>
+                  <c:v>0.21199999999999999</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>0.22</c:v>
+                  <c:v>0.22500000000000001</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>0.25</c:v>
+                  <c:v>0.22800000000000001</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.22</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>0.23</c:v>
+                  <c:v>0.224</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8790,9 +8771,6 @@
                 <c:pt idx="98">
                   <c:v>990000</c:v>
                 </c:pt>
-                <c:pt idx="99">
-                  <c:v>1000000</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -8806,301 +8784,298 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.01</c:v>
+                  <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>4.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>4.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>5.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.01</c:v>
+                  <c:v>6.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.01</c:v>
+                  <c:v>6.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.01</c:v>
+                  <c:v>7.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.01</c:v>
+                  <c:v>8.0000000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.01</c:v>
+                  <c:v>8.0000000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.01</c:v>
+                  <c:v>8.9999999999999993E-3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.01</c:v>
+                  <c:v>8.9999999999999993E-3</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.01</c:v>
+                  <c:v>1.0999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.01</c:v>
+                  <c:v>1.2E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.01</c:v>
+                  <c:v>1.6E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.01</c:v>
+                  <c:v>1.4E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.01</c:v>
+                  <c:v>1.4E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.02</c:v>
+                  <c:v>1.6E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.02</c:v>
+                  <c:v>1.9E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.01</c:v>
+                  <c:v>1.6E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.02</c:v>
+                  <c:v>1.7000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.01</c:v>
+                  <c:v>2.1999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.01</c:v>
+                  <c:v>1.7000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.02</c:v>
+                  <c:v>1.7000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.03</c:v>
+                  <c:v>1.7999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.02</c:v>
+                  <c:v>2.1000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.02</c:v>
+                  <c:v>3.7999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.02</c:v>
+                  <c:v>2.1999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.02</c:v>
+                  <c:v>2.3E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.02</c:v>
+                  <c:v>2.4E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.02</c:v>
+                  <c:v>3.1E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.03</c:v>
+                  <c:v>2.5000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.02</c:v>
+                  <c:v>2.5999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.03</c:v>
+                  <c:v>2.5999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.03</c:v>
+                  <c:v>2.7E-2</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.03</c:v>
+                  <c:v>2.9000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
                   <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="43">
+                  <c:v>3.2000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3.9E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3.4000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
                   <c:v>0.04</c:v>
                 </c:pt>
-                <c:pt idx="44">
-                  <c:v>0.04</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.03</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>0.03</c:v>
-                </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.05</c:v>
+                  <c:v>5.2999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.03</c:v>
+                  <c:v>3.6999999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.03</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.04</c:v>
+                  <c:v>5.1999999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.05</c:v>
+                  <c:v>5.1999999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>0.04</c:v>
+                  <c:v>4.5999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="54">
+                  <c:v>5.5E-2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>6.5000000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>5.0999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5.8999999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>6.0999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="59">
                   <c:v>0.06</c:v>
                 </c:pt>
-                <c:pt idx="55">
-                  <c:v>0.04</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>7.0000000000000007E-2</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>0.06</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>0.06</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>7.0000000000000007E-2</c:v>
-                </c:pt>
                 <c:pt idx="60">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>7.5999999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>6.0999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="62">
                   <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.06</c:v>
+                  <c:v>7.9000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>8.4000000000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.06</c:v>
+                  <c:v>7.0999999999999994E-2</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>6.9000000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>6.6000000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>6.5000000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.08</c:v>
+                  <c:v>7.6999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.08</c:v>
+                  <c:v>8.6999999999999994E-2</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.08</c:v>
+                  <c:v>7.9000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.09</c:v>
+                  <c:v>8.5999999999999993E-2</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.08</c:v>
+                  <c:v>0.10299999999999999</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.08</c:v>
+                  <c:v>8.2000000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.11</c:v>
+                  <c:v>8.5999999999999993E-2</c:v>
                 </c:pt>
                 <c:pt idx="76">
+                  <c:v>8.3000000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>8.8999999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>8.8999999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="79">
                   <c:v>0.1</c:v>
                 </c:pt>
-                <c:pt idx="77">
-                  <c:v>0.08</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>0.09</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>0.11</c:v>
-                </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.12</c:v>
+                  <c:v>0.10299999999999999</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.09</c:v>
+                  <c:v>9.7000000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.11</c:v>
+                  <c:v>9.8000000000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.12</c:v>
+                  <c:v>0.10299999999999999</c:v>
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.12</c:v>
+                  <c:v>0.10100000000000001</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.14000000000000001</c:v>
+                  <c:v>0.127</c:v>
                 </c:pt>
                 <c:pt idx="87">
+                  <c:v>0.121</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.113</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.111</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.113</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.109</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.113</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.11799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.123</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="97">
                   <c:v>0.13</c:v>
                 </c:pt>
-                <c:pt idx="88">
-                  <c:v>0.11</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>0.11</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>0.14000000000000001</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>0.14000000000000001</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>0.15</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>0.11</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>0.15</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>0.13</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>0.16</c:v>
-                </c:pt>
                 <c:pt idx="98">
-                  <c:v>0.12</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>0.13</c:v>
+                  <c:v>0.121</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9115,11 +9090,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="82235392"/>
-        <c:axId val="82213120"/>
+        <c:axId val="132088576"/>
+        <c:axId val="132090112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="82235392"/>
+        <c:axId val="132088576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9129,12 +9104,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82213120"/>
+        <c:crossAx val="132090112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="82213120"/>
+        <c:axId val="132090112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9145,7 +9120,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82235392"/>
+        <c:crossAx val="132088576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -15254,10 +15229,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I101"/>
+  <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -15287,13 +15262,13 @@
         <v>10000</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="D2">
-        <v>0.01</v>
+        <v>2E-3</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -15304,16 +15279,16 @@
         <v>20000</v>
       </c>
       <c r="B3">
-        <v>0.01</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="D3">
-        <v>0.01</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>2E-3</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
@@ -15321,16 +15296,16 @@
         <v>30000</v>
       </c>
       <c r="B4">
-        <v>0.01</v>
+        <v>1.2E-2</v>
       </c>
       <c r="C4">
-        <v>0.01</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>2E-3</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
@@ -15338,16 +15313,16 @@
         <v>40000</v>
       </c>
       <c r="B5">
-        <v>0.01</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>2E-3</v>
       </c>
       <c r="D5">
-        <v>0.01</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>3.0000000000000001E-3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.15">
@@ -15355,16 +15330,16 @@
         <v>50000</v>
       </c>
       <c r="B6">
-        <v>0.01</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="C6">
-        <v>0.01</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D6">
-        <v>0.01</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>3.0000000000000001E-3</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.15">
@@ -15372,16 +15347,16 @@
         <v>60000</v>
       </c>
       <c r="B7">
-        <v>0.02</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D7">
         <v>0.01</v>
       </c>
       <c r="E7">
-        <v>0.01</v>
+        <v>3.0000000000000001E-3</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
@@ -15389,16 +15364,16 @@
         <v>70000</v>
       </c>
       <c r="B8">
-        <v>0.02</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="C8">
-        <v>0.01</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D8">
-        <v>0.02</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
@@ -15406,16 +15381,16 @@
         <v>80000</v>
       </c>
       <c r="B9">
-        <v>0.02</v>
+        <v>3.1E-2</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D9">
-        <v>0.02</v>
+        <v>1.6E-2</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.15">
@@ -15423,16 +15398,16 @@
         <v>90000</v>
       </c>
       <c r="B10">
-        <v>0.02</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="C10">
-        <v>0.01</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="D10">
-        <v>0.02</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.15">
@@ -15440,16 +15415,16 @@
         <v>100000</v>
       </c>
       <c r="B11">
-        <v>0.03</v>
+        <v>4.7E-2</v>
       </c>
       <c r="C11">
-        <v>0.01</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="D11">
-        <v>0.02</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="E11">
-        <v>0.01</v>
+        <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.15">
@@ -15457,16 +15432,16 @@
         <v>110000</v>
       </c>
       <c r="B12">
-        <v>0.03</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="D12">
-        <v>0.02</v>
+        <v>1.9E-2</v>
       </c>
       <c r="E12">
-        <v>0.01</v>
+        <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.15">
@@ -15477,13 +15452,13 @@
         <v>0.04</v>
       </c>
       <c r="C13">
-        <v>0.01</v>
+        <v>1.2E-2</v>
       </c>
       <c r="D13">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="E13">
-        <v>0.01</v>
+        <v>7.0000000000000001E-3</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.15">
@@ -15491,16 +15466,16 @@
         <v>130000</v>
       </c>
       <c r="B14">
-        <v>0.04</v>
+        <v>7.3999999999999996E-2</v>
       </c>
       <c r="C14">
-        <v>0.01</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="D14">
-        <v>0.02</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="E14">
-        <v>0.01</v>
+        <v>8.0000000000000002E-3</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.15">
@@ -15508,16 +15483,16 @@
         <v>140000</v>
       </c>
       <c r="B15">
-        <v>0.04</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="C15">
         <v>0.01</v>
       </c>
       <c r="D15">
-        <v>0.04</v>
+        <v>3.1E-2</v>
       </c>
       <c r="E15">
-        <v>0.01</v>
+        <v>8.0000000000000002E-3</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.15">
@@ -15525,13 +15500,13 @@
         <v>150000</v>
       </c>
       <c r="B16">
-        <v>0.04</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="C16">
         <v>0.01</v>
       </c>
       <c r="D16">
-        <v>0.03</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="E16">
         <v>0.01</v>
@@ -15542,16 +15517,16 @@
         <v>160000</v>
       </c>
       <c r="B17">
-        <v>0.05</v>
+        <v>5.8999999999999997E-2</v>
       </c>
       <c r="C17">
-        <v>0.01</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="D17">
-        <v>0.04</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="E17">
-        <v>0.01</v>
+        <v>8.9999999999999993E-3</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.15">
@@ -15559,16 +15534,16 @@
         <v>170000</v>
       </c>
       <c r="B18">
-        <v>0.05</v>
+        <v>6.2E-2</v>
       </c>
       <c r="C18">
-        <v>0.02</v>
+        <v>1.2E-2</v>
       </c>
       <c r="D18">
-        <v>0.03</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="E18">
-        <v>0.01</v>
+        <v>8.9999999999999993E-3</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.15">
@@ -15576,13 +15551,13 @@
         <v>180000</v>
       </c>
       <c r="B19">
-        <v>0.05</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="C19">
-        <v>0.01</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="D19">
-        <v>0.03</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="E19">
         <v>0.01</v>
@@ -15593,16 +15568,16 @@
         <v>190000</v>
       </c>
       <c r="B20">
-        <v>0.06</v>
+        <v>0.08</v>
       </c>
       <c r="C20">
-        <v>0.01</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D20">
-        <v>0.04</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="E20">
-        <v>0.01</v>
+        <v>1.0999999999999999E-2</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.15">
@@ -15610,16 +15585,16 @@
         <v>200000</v>
       </c>
       <c r="B21">
-        <v>0.06</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="C21">
-        <v>0.01</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="D21">
-        <v>0.04</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="E21">
-        <v>0.01</v>
+        <v>1.2E-2</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
@@ -15627,16 +15602,16 @@
         <v>210000</v>
       </c>
       <c r="B22">
-        <v>0.06</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="C22">
-        <v>0.02</v>
+        <v>1.9E-2</v>
       </c>
       <c r="D22">
-        <v>0.04</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="E22">
-        <v>0.01</v>
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
@@ -15644,16 +15619,16 @@
         <v>220000</v>
       </c>
       <c r="B23">
-        <v>0.06</v>
+        <v>7.8E-2</v>
       </c>
       <c r="C23">
-        <v>0.02</v>
+        <v>2.7E-2</v>
       </c>
       <c r="D23">
-        <v>0.04</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="E23">
-        <v>0.01</v>
+        <v>1.4E-2</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
@@ -15661,16 +15636,16 @@
         <v>230000</v>
       </c>
       <c r="B24">
-        <v>0.06</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="C24">
-        <v>0.02</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="D24">
-        <v>0.04</v>
+        <v>3.9E-2</v>
       </c>
       <c r="E24">
-        <v>0.01</v>
+        <v>1.4E-2</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
@@ -15678,16 +15653,16 @@
         <v>240000</v>
       </c>
       <c r="B25">
-        <v>7.0000000000000007E-2</v>
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="C25">
-        <v>0.02</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="D25">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="E25">
-        <v>0.02</v>
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
@@ -15695,16 +15670,16 @@
         <v>250000</v>
       </c>
       <c r="B26">
-        <v>0.09</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="C26">
-        <v>0.02</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D26">
-        <v>0.04</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="E26">
-        <v>0.02</v>
+        <v>1.9E-2</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
@@ -15712,16 +15687,16 @@
         <v>260000</v>
       </c>
       <c r="B27">
-        <v>0.1</v>
+        <v>0.128</v>
       </c>
       <c r="C27">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="D27">
-        <v>0.05</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="E27">
-        <v>0.01</v>
+        <v>1.6E-2</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
@@ -15729,16 +15704,16 @@
         <v>270000</v>
       </c>
       <c r="B28">
-        <v>0.1</v>
+        <v>0.124</v>
       </c>
       <c r="C28">
-        <v>0.03</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="D28">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="E28">
-        <v>0.02</v>
+        <v>1.7000000000000001E-2</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
@@ -15746,16 +15721,16 @@
         <v>280000</v>
       </c>
       <c r="B29">
-        <v>0.11</v>
+        <v>0.126</v>
       </c>
       <c r="C29">
-        <v>0.03</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="D29">
-        <v>0.06</v>
+        <v>6.2E-2</v>
       </c>
       <c r="E29">
-        <v>0.01</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
@@ -15763,16 +15738,16 @@
         <v>290000</v>
       </c>
       <c r="B30">
-        <v>0.1</v>
+        <v>0.122</v>
       </c>
       <c r="C30">
-        <v>0.03</v>
+        <v>3.1E-2</v>
       </c>
       <c r="D30">
-        <v>7.0000000000000007E-2</v>
+        <v>6.3E-2</v>
       </c>
       <c r="E30">
-        <v>0.01</v>
+        <v>1.7000000000000001E-2</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
@@ -15780,16 +15755,16 @@
         <v>300000</v>
       </c>
       <c r="B31">
-        <v>0.11</v>
+        <v>0.127</v>
       </c>
       <c r="C31">
-        <v>0.03</v>
+        <v>3.1E-2</v>
       </c>
       <c r="D31">
-        <v>0.06</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="E31">
-        <v>0.02</v>
+        <v>1.7000000000000001E-2</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
@@ -15797,16 +15772,16 @@
         <v>310000</v>
       </c>
       <c r="B32">
-        <v>0.11</v>
+        <v>0.127</v>
       </c>
       <c r="C32">
-        <v>0.03</v>
+        <v>2.9000000000000001E-2</v>
       </c>
       <c r="D32">
-        <v>7.0000000000000007E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="E32">
-        <v>0.03</v>
+        <v>1.7999999999999999E-2</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
@@ -15814,16 +15789,16 @@
         <v>320000</v>
       </c>
       <c r="B33">
-        <v>0.18</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="C33">
-        <v>0.06</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="D33">
-        <v>7.0000000000000007E-2</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="E33">
-        <v>0.02</v>
+        <v>2.1000000000000001E-2</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.15">
@@ -15831,16 +15806,16 @@
         <v>330000</v>
       </c>
       <c r="B34">
-        <v>0.11</v>
+        <v>0.14699999999999999</v>
       </c>
       <c r="C34">
-        <v>0.04</v>
+        <v>3.9E-2</v>
       </c>
       <c r="D34">
-        <v>0.06</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="E34">
-        <v>0.02</v>
+        <v>3.7999999999999999E-2</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.15">
@@ -15848,16 +15823,16 @@
         <v>340000</v>
       </c>
       <c r="B35">
-        <v>0.13</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="C35">
-        <v>0.04</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="D35">
-        <v>0.06</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="E35">
-        <v>0.02</v>
+        <v>2.1999999999999999E-2</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.15">
@@ -15865,16 +15840,16 @@
         <v>350000</v>
       </c>
       <c r="B36">
-        <v>0.13</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="C36">
-        <v>0.03</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="D36">
-        <v>7.0000000000000007E-2</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="E36">
-        <v>0.02</v>
+        <v>2.3E-2</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.15">
@@ -15882,16 +15857,16 @@
         <v>360000</v>
       </c>
       <c r="B37">
-        <v>0.12</v>
+        <v>0.154</v>
       </c>
       <c r="C37">
         <v>0.04</v>
       </c>
       <c r="D37">
-        <v>0.08</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="E37">
-        <v>0.02</v>
+        <v>2.4E-2</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.15">
@@ -15899,16 +15874,16 @@
         <v>370000</v>
       </c>
       <c r="B38">
-        <v>0.13</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="C38">
-        <v>0.04</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="D38">
-        <v>0.08</v>
+        <v>7.3999999999999996E-2</v>
       </c>
       <c r="E38">
-        <v>0.02</v>
+        <v>3.1E-2</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.15">
@@ -15916,16 +15891,16 @@
         <v>380000</v>
       </c>
       <c r="B39">
-        <v>0.13</v>
+        <v>0.154</v>
       </c>
       <c r="C39">
-        <v>0.04</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="D39">
-        <v>0.08</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="E39">
-        <v>0.03</v>
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.15">
@@ -15933,16 +15908,16 @@
         <v>390000</v>
       </c>
       <c r="B40">
-        <v>0.13</v>
+        <v>0.16400000000000001</v>
       </c>
       <c r="C40">
-        <v>0.04</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="D40">
-        <v>0.08</v>
+        <v>7.9000000000000001E-2</v>
       </c>
       <c r="E40">
-        <v>0.02</v>
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.15">
@@ -15950,16 +15925,16 @@
         <v>400000</v>
       </c>
       <c r="B41">
-        <v>0.14000000000000001</v>
+        <v>0.155</v>
       </c>
       <c r="C41">
-        <v>0.05</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="D41">
-        <v>0.08</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="E41">
-        <v>0.03</v>
+        <v>2.5999999999999999E-2</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
@@ -15967,16 +15942,16 @@
         <v>410000</v>
       </c>
       <c r="B42">
-        <v>0.14000000000000001</v>
+        <v>0.16900000000000001</v>
       </c>
       <c r="C42">
-        <v>0.06</v>
+        <v>0.05</v>
       </c>
       <c r="D42">
-        <v>7.0000000000000007E-2</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="E42">
-        <v>0.03</v>
+        <v>2.7E-2</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.15">
@@ -15984,7 +15959,7 @@
         <v>420000</v>
       </c>
       <c r="B43">
-        <v>0.15</v>
+        <v>0.17100000000000001</v>
       </c>
       <c r="C43">
         <v>0.05</v>
@@ -15993,7 +15968,7 @@
         <v>0.08</v>
       </c>
       <c r="E43">
-        <v>0.03</v>
+        <v>2.9000000000000001E-2</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.15">
@@ -16001,13 +15976,13 @@
         <v>430000</v>
       </c>
       <c r="B44">
-        <v>0.15</v>
+        <v>0.18</v>
       </c>
       <c r="C44">
         <v>0.05</v>
       </c>
       <c r="D44">
-        <v>0.08</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="E44">
         <v>0.03</v>
@@ -16018,16 +15993,16 @@
         <v>440000</v>
       </c>
       <c r="B45">
-        <v>0.16</v>
+        <v>0.17599999999999999</v>
       </c>
       <c r="C45">
         <v>0.05</v>
       </c>
       <c r="D45">
-        <v>7.0000000000000007E-2</v>
+        <v>0.08</v>
       </c>
       <c r="E45">
-        <v>0.04</v>
+        <v>3.2000000000000001E-2</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.15">
@@ -16035,16 +16010,16 @@
         <v>450000</v>
       </c>
       <c r="B46">
-        <v>0.16</v>
+        <v>0.17799999999999999</v>
       </c>
       <c r="C46">
-        <v>0.05</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="D46">
-        <v>0.09</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="E46">
-        <v>0.04</v>
+        <v>3.9E-2</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.15">
@@ -16052,16 +16027,16 @@
         <v>460000</v>
       </c>
       <c r="B47">
-        <v>0.15</v>
+        <v>0.184</v>
       </c>
       <c r="C47">
-        <v>0.06</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="D47">
-        <v>0.08</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="E47">
-        <v>0.03</v>
+        <v>3.4000000000000002E-2</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.15">
@@ -16069,16 +16044,16 @@
         <v>470000</v>
       </c>
       <c r="B48">
-        <v>0.17</v>
+        <v>0.182</v>
       </c>
       <c r="C48">
-        <v>0.05</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="D48">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="E48">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.15">
@@ -16086,16 +16061,16 @@
         <v>480000</v>
       </c>
       <c r="B49">
-        <v>0.17</v>
+        <v>0.19</v>
       </c>
       <c r="C49">
-        <v>0.06</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="D49">
-        <v>0.09</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="E49">
-        <v>0.05</v>
+        <v>5.2999999999999999E-2</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.15">
@@ -16103,13 +16078,13 @@
         <v>490000</v>
       </c>
       <c r="B50">
-        <v>0.18</v>
+        <v>0.186</v>
       </c>
       <c r="C50">
-        <v>0.06</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="D50">
-        <v>0.08</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="E50">
         <v>0.04</v>
@@ -16120,16 +16095,16 @@
         <v>500000</v>
       </c>
       <c r="B51">
-        <v>0.18</v>
+        <v>0.191</v>
       </c>
       <c r="C51">
-        <v>0.06</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="D51">
-        <v>0.1</v>
+        <v>9.1999999999999998E-2</v>
       </c>
       <c r="E51">
-        <v>0.03</v>
+        <v>3.6999999999999998E-2</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.15">
@@ -16137,16 +16112,16 @@
         <v>510000</v>
       </c>
       <c r="B52">
-        <v>0.17</v>
+        <v>0.19500000000000001</v>
       </c>
       <c r="C52">
-        <v>7.0000000000000007E-2</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="D52">
-        <v>0.09</v>
+        <v>0.10299999999999999</v>
       </c>
       <c r="E52">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.15">
@@ -16154,16 +16129,16 @@
         <v>520000</v>
       </c>
       <c r="B53">
-        <v>0.18</v>
+        <v>0.20300000000000001</v>
       </c>
       <c r="C53">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="D53">
-        <v>0.1</v>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="E53">
-        <v>0.04</v>
+        <v>5.1999999999999998E-2</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.15">
@@ -16171,16 +16146,16 @@
         <v>530000</v>
       </c>
       <c r="B54">
-        <v>0.24</v>
+        <v>0.25900000000000001</v>
       </c>
       <c r="C54">
-        <v>0.06</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="D54">
-        <v>0.15</v>
+        <v>0.13600000000000001</v>
       </c>
       <c r="E54">
-        <v>0.05</v>
+        <v>5.1999999999999998E-2</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.15">
@@ -16188,16 +16163,16 @@
         <v>540000</v>
       </c>
       <c r="B55">
-        <v>0.26</v>
+        <v>0.27500000000000002</v>
       </c>
       <c r="C55">
-        <v>7.0000000000000007E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="D55">
-        <v>0.14000000000000001</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="E55">
-        <v>0.04</v>
+        <v>4.5999999999999999E-2</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.15">
@@ -16205,16 +16180,16 @@
         <v>550000</v>
       </c>
       <c r="B56">
-        <v>0.25</v>
+        <v>0.27600000000000002</v>
       </c>
       <c r="C56">
-        <v>7.0000000000000007E-2</v>
+        <v>6.9000000000000006E-2</v>
       </c>
       <c r="D56">
-        <v>0.14000000000000001</v>
+        <v>0.14199999999999999</v>
       </c>
       <c r="E56">
-        <v>0.06</v>
+        <v>5.5E-2</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.15">
@@ -16222,16 +16197,16 @@
         <v>560000</v>
       </c>
       <c r="B57">
-        <v>0.27</v>
+        <v>0.28100000000000003</v>
       </c>
       <c r="C57">
-        <v>0.06</v>
+        <v>6.7000000000000004E-2</v>
       </c>
       <c r="D57">
-        <v>0.15</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="E57">
-        <v>0.04</v>
+        <v>6.5000000000000002E-2</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.15">
@@ -16239,16 +16214,16 @@
         <v>570000</v>
       </c>
       <c r="B58">
-        <v>0.27</v>
+        <v>0.28799999999999998</v>
       </c>
       <c r="C58">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="D58">
-        <v>0.15</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="E58">
-        <v>7.0000000000000007E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.15">
@@ -16256,16 +16231,16 @@
         <v>580000</v>
       </c>
       <c r="B59">
-        <v>0.27</v>
+        <v>0.27800000000000002</v>
       </c>
       <c r="C59">
-        <v>7.0000000000000007E-2</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="D59">
-        <v>0.15</v>
+        <v>0.14699999999999999</v>
       </c>
       <c r="E59">
-        <v>0.06</v>
+        <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.15">
@@ -16276,13 +16251,13 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="C60">
-        <v>0.08</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="D60">
-        <v>0.15</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="E60">
-        <v>0.06</v>
+        <v>6.0999999999999999E-2</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.15">
@@ -16290,16 +16265,16 @@
         <v>600000</v>
       </c>
       <c r="B61">
-        <v>0.28999999999999998</v>
+        <v>0.32200000000000001</v>
       </c>
       <c r="C61">
-        <v>7.0000000000000007E-2</v>
+        <v>7.3999999999999996E-2</v>
       </c>
       <c r="D61">
-        <v>0.16</v>
+        <v>0.153</v>
       </c>
       <c r="E61">
-        <v>7.0000000000000007E-2</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.15">
@@ -16307,16 +16282,16 @@
         <v>610000</v>
       </c>
       <c r="B62">
-        <v>0.28999999999999998</v>
+        <v>0.30399999999999999</v>
       </c>
       <c r="C62">
-        <v>0.08</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="D62">
-        <v>0.16</v>
+        <v>0.158</v>
       </c>
       <c r="E62">
-        <v>7.0000000000000007E-2</v>
+        <v>7.5999999999999998E-2</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.15">
@@ -16324,16 +16299,16 @@
         <v>620000</v>
       </c>
       <c r="B63">
-        <v>0.26</v>
+        <v>0.29599999999999999</v>
       </c>
       <c r="C63">
         <v>0.08</v>
       </c>
       <c r="D63">
-        <v>0.15</v>
+        <v>0.152</v>
       </c>
       <c r="E63">
-        <v>7.0000000000000007E-2</v>
+        <v>6.0999999999999999E-2</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.15">
@@ -16341,13 +16316,13 @@
         <v>630000</v>
       </c>
       <c r="B64">
-        <v>0.27</v>
+        <v>0.29899999999999999</v>
       </c>
       <c r="C64">
-        <v>0.08</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="D64">
-        <v>0.16</v>
+        <v>0.14699999999999999</v>
       </c>
       <c r="E64">
         <v>0.06</v>
@@ -16358,16 +16333,16 @@
         <v>640000</v>
       </c>
       <c r="B65">
-        <v>0.28999999999999998</v>
+        <v>0.316</v>
       </c>
       <c r="C65">
-        <v>0.08</v>
+        <v>8.3000000000000004E-2</v>
       </c>
       <c r="D65">
-        <v>0.15</v>
+        <v>0.156</v>
       </c>
       <c r="E65">
-        <v>0.06</v>
+        <v>7.9000000000000001E-2</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.15">
@@ -16375,16 +16350,16 @@
         <v>650000</v>
       </c>
       <c r="B66">
-        <v>0.31</v>
+        <v>0.30299999999999999</v>
       </c>
       <c r="C66">
-        <v>0.08</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="D66">
-        <v>0.15</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="E66">
-        <v>7.0000000000000007E-2</v>
+        <v>8.4000000000000005E-2</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.15">
@@ -16392,16 +16367,16 @@
         <v>660000</v>
       </c>
       <c r="B67">
-        <v>0.28000000000000003</v>
+        <v>0.30599999999999999</v>
       </c>
       <c r="C67">
-        <v>0.09</v>
+        <v>9.4E-2</v>
       </c>
       <c r="D67">
-        <v>0.16</v>
+        <v>0.153</v>
       </c>
       <c r="E67">
-        <v>0.06</v>
+        <v>7.0999999999999994E-2</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.15">
@@ -16409,16 +16384,16 @@
         <v>670000</v>
       </c>
       <c r="B68">
-        <v>0.32</v>
+        <v>0.311</v>
       </c>
       <c r="C68">
-        <v>0.08</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="D68">
-        <v>0.15</v>
+        <v>0.16200000000000001</v>
       </c>
       <c r="E68">
-        <v>7.0000000000000007E-2</v>
+        <v>6.9000000000000006E-2</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.15">
@@ -16426,16 +16401,16 @@
         <v>680000</v>
       </c>
       <c r="B69">
-        <v>0.28999999999999998</v>
+        <v>0.33100000000000002</v>
       </c>
       <c r="C69">
-        <v>0.1</v>
+        <v>0.09</v>
       </c>
       <c r="D69">
-        <v>0.16</v>
+        <v>0.16300000000000001</v>
       </c>
       <c r="E69">
-        <v>7.0000000000000007E-2</v>
+        <v>6.6000000000000003E-2</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.15">
@@ -16443,16 +16418,16 @@
         <v>690000</v>
       </c>
       <c r="B70">
-        <v>0.31</v>
+        <v>0.317</v>
       </c>
       <c r="C70">
-        <v>0.1</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="D70">
-        <v>0.17</v>
+        <v>0.161</v>
       </c>
       <c r="E70">
-        <v>7.0000000000000007E-2</v>
+        <v>6.5000000000000002E-2</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.15">
@@ -16460,16 +16435,16 @@
         <v>700000</v>
       </c>
       <c r="B71">
-        <v>0.3</v>
+        <v>0.31900000000000001</v>
       </c>
       <c r="C71">
-        <v>0.09</v>
+        <v>9.4E-2</v>
       </c>
       <c r="D71">
-        <v>0.16</v>
+        <v>0.182</v>
       </c>
       <c r="E71">
-        <v>0.08</v>
+        <v>7.6999999999999999E-2</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.15">
@@ -16477,16 +16452,16 @@
         <v>710000</v>
       </c>
       <c r="B72">
-        <v>0.31</v>
+        <v>0.318</v>
       </c>
       <c r="C72">
-        <v>0.1</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="D72">
-        <v>0.19</v>
+        <v>0.16600000000000001</v>
       </c>
       <c r="E72">
-        <v>0.08</v>
+        <v>8.6999999999999994E-2</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.15">
@@ -16494,16 +16469,16 @@
         <v>720000</v>
       </c>
       <c r="B73">
-        <v>0.31</v>
+        <v>0.32900000000000001</v>
       </c>
       <c r="C73">
-        <v>0.09</v>
+        <v>0.104</v>
       </c>
       <c r="D73">
-        <v>0.17</v>
+        <v>0.17199999999999999</v>
       </c>
       <c r="E73">
-        <v>0.08</v>
+        <v>7.9000000000000001E-2</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.15">
@@ -16511,16 +16486,16 @@
         <v>730000</v>
       </c>
       <c r="B74">
-        <v>0.33</v>
+        <v>0.34300000000000003</v>
       </c>
       <c r="C74">
-        <v>0.11</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="D74">
-        <v>0.19</v>
+        <v>0.16900000000000001</v>
       </c>
       <c r="E74">
-        <v>0.09</v>
+        <v>8.5999999999999993E-2</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.15">
@@ -16528,16 +16503,16 @@
         <v>740000</v>
       </c>
       <c r="B75">
-        <v>0.32</v>
+        <v>0.33600000000000002</v>
       </c>
       <c r="C75">
-        <v>0.11</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="D75">
-        <v>0.17</v>
+        <v>0.18</v>
       </c>
       <c r="E75">
-        <v>0.08</v>
+        <v>0.10299999999999999</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.15">
@@ -16545,16 +16520,16 @@
         <v>750000</v>
       </c>
       <c r="B76">
-        <v>0.31</v>
+        <v>0.34200000000000003</v>
       </c>
       <c r="C76">
-        <v>0.1</v>
+        <v>0.10199999999999999</v>
       </c>
       <c r="D76">
-        <v>0.17</v>
+        <v>0.17399999999999999</v>
       </c>
       <c r="E76">
-        <v>0.08</v>
+        <v>8.2000000000000003E-2</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.15">
@@ -16562,16 +16537,16 @@
         <v>760000</v>
       </c>
       <c r="B77">
-        <v>0.35</v>
+        <v>0.35399999999999998</v>
       </c>
       <c r="C77">
-        <v>0.12</v>
+        <v>0.106</v>
       </c>
       <c r="D77">
-        <v>0.2</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="E77">
-        <v>0.11</v>
+        <v>8.5999999999999993E-2</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.15">
@@ -16579,16 +16554,16 @@
         <v>770000</v>
       </c>
       <c r="B78">
-        <v>0.34</v>
+        <v>0.35</v>
       </c>
       <c r="C78">
-        <v>0.12</v>
+        <v>0.11799999999999999</v>
       </c>
       <c r="D78">
-        <v>0.19</v>
+        <v>0.17899999999999999</v>
       </c>
       <c r="E78">
-        <v>0.1</v>
+        <v>8.3000000000000004E-2</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.15">
@@ -16596,16 +16571,16 @@
         <v>780000</v>
       </c>
       <c r="B79">
-        <v>0.35</v>
+        <v>0.36</v>
       </c>
       <c r="C79">
-        <v>0.12</v>
+        <v>0.107</v>
       </c>
       <c r="D79">
-        <v>0.2</v>
+        <v>0.19600000000000001</v>
       </c>
       <c r="E79">
-        <v>0.08</v>
+        <v>8.8999999999999996E-2</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.15">
@@ -16613,16 +16588,16 @@
         <v>790000</v>
       </c>
       <c r="B80">
-        <v>0.34</v>
+        <v>0.34499999999999997</v>
       </c>
       <c r="C80">
-        <v>0.11</v>
+        <v>0.108</v>
       </c>
       <c r="D80">
-        <v>0.2</v>
+        <v>0.19</v>
       </c>
       <c r="E80">
-        <v>0.09</v>
+        <v>8.8999999999999996E-2</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.15">
@@ -16630,16 +16605,16 @@
         <v>800000</v>
       </c>
       <c r="B81">
-        <v>0.33</v>
+        <v>0.34699999999999998</v>
       </c>
       <c r="C81">
-        <v>0.11</v>
+        <v>0.111</v>
       </c>
       <c r="D81">
-        <v>0.19</v>
+        <v>0.185</v>
       </c>
       <c r="E81">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.15">
@@ -16647,16 +16622,16 @@
         <v>810000</v>
       </c>
       <c r="B82">
-        <v>0.36</v>
+        <v>0.36599999999999999</v>
       </c>
       <c r="C82">
-        <v>0.12</v>
+        <v>0.115</v>
       </c>
       <c r="D82">
-        <v>0.18</v>
+        <v>0.17599999999999999</v>
       </c>
       <c r="E82">
-        <v>0.12</v>
+        <v>0.10299999999999999</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.15">
@@ -16664,16 +16639,16 @@
         <v>820000</v>
       </c>
       <c r="B83">
-        <v>0.35</v>
+        <v>0.36399999999999999</v>
       </c>
       <c r="C83">
-        <v>0.13</v>
+        <v>0.124</v>
       </c>
       <c r="D83">
-        <v>0.18</v>
+        <v>0.189</v>
       </c>
       <c r="E83">
-        <v>0.09</v>
+        <v>9.7000000000000003E-2</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.15">
@@ -16681,16 +16656,16 @@
         <v>830000</v>
       </c>
       <c r="B84">
-        <v>0.36</v>
+        <v>0.36399999999999999</v>
       </c>
       <c r="C84">
-        <v>0.13</v>
+        <v>0.11799999999999999</v>
       </c>
       <c r="D84">
-        <v>0.19</v>
+        <v>0.193</v>
       </c>
       <c r="E84">
-        <v>0.11</v>
+        <v>9.8000000000000004E-2</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.15">
@@ -16698,16 +16673,16 @@
         <v>840000</v>
       </c>
       <c r="B85">
-        <v>0.34</v>
+        <v>0.36399999999999999</v>
       </c>
       <c r="C85">
-        <v>0.12</v>
+        <v>0.11899999999999999</v>
       </c>
       <c r="D85">
-        <v>0.19</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="E85">
-        <v>0.12</v>
+        <v>0.10299999999999999</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.15">
@@ -16715,10 +16690,10 @@
         <v>850000</v>
       </c>
       <c r="B86">
-        <v>0.36</v>
+        <v>0.36899999999999999</v>
       </c>
       <c r="C86">
-        <v>0.12</v>
+        <v>0.13100000000000001</v>
       </c>
       <c r="D86">
         <v>0.19</v>
@@ -16732,16 +16707,16 @@
         <v>860000</v>
       </c>
       <c r="B87">
-        <v>0.37</v>
+        <v>0.38800000000000001</v>
       </c>
       <c r="C87">
-        <v>0.12</v>
+        <v>0.121</v>
       </c>
       <c r="D87">
-        <v>0.19</v>
+        <v>0.191</v>
       </c>
       <c r="E87">
-        <v>0.12</v>
+        <v>0.10100000000000001</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.15">
@@ -16749,16 +16724,16 @@
         <v>870000</v>
       </c>
       <c r="B88">
-        <v>0.4</v>
+        <v>0.38500000000000001</v>
       </c>
       <c r="C88">
-        <v>0.14000000000000001</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="D88">
-        <v>0.23</v>
+        <v>0.20300000000000001</v>
       </c>
       <c r="E88">
-        <v>0.14000000000000001</v>
+        <v>0.127</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.15">
@@ -16766,16 +16741,16 @@
         <v>880000</v>
       </c>
       <c r="B89">
-        <v>0.37</v>
+        <v>0.38200000000000001</v>
       </c>
       <c r="C89">
-        <v>0.14000000000000001</v>
+        <v>0.128</v>
       </c>
       <c r="D89">
-        <v>0.2</v>
+        <v>0.19800000000000001</v>
       </c>
       <c r="E89">
-        <v>0.13</v>
+        <v>0.121</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.15">
@@ -16783,16 +16758,16 @@
         <v>890000</v>
       </c>
       <c r="B90">
-        <v>0.39</v>
+        <v>0.378</v>
       </c>
       <c r="C90">
-        <v>0.15</v>
+        <v>0.13</v>
       </c>
       <c r="D90">
-        <v>0.19</v>
+        <v>0.20100000000000001</v>
       </c>
       <c r="E90">
-        <v>0.11</v>
+        <v>0.113</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.15">
@@ -16800,16 +16775,16 @@
         <v>900000</v>
       </c>
       <c r="B91">
-        <v>0.38</v>
+        <v>0.38700000000000001</v>
       </c>
       <c r="C91">
-        <v>0.14000000000000001</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="D91">
-        <v>0.2</v>
+        <v>0.217</v>
       </c>
       <c r="E91">
-        <v>0.11</v>
+        <v>0.111</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.15">
@@ -16817,16 +16792,16 @@
         <v>910000</v>
       </c>
       <c r="B92">
-        <v>0.41</v>
+        <v>0.40200000000000002</v>
       </c>
       <c r="C92">
-        <v>0.15</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="D92">
-        <v>0.24</v>
+        <v>0.21</v>
       </c>
       <c r="E92">
-        <v>0.14000000000000001</v>
+        <v>0.113</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.15">
@@ -16834,16 +16809,16 @@
         <v>920000</v>
       </c>
       <c r="B93">
-        <v>0.38</v>
+        <v>0.39500000000000002</v>
       </c>
       <c r="C93">
-        <v>0.14000000000000001</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="D93">
-        <v>0.23</v>
+        <v>0.20899999999999999</v>
       </c>
       <c r="E93">
-        <v>0.14000000000000001</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.15">
@@ -16851,16 +16826,16 @@
         <v>930000</v>
       </c>
       <c r="B94">
-        <v>0.38</v>
+        <v>0.39600000000000002</v>
       </c>
       <c r="C94">
-        <v>0.15</v>
+        <v>0.14099999999999999</v>
       </c>
       <c r="D94">
-        <v>0.25</v>
+        <v>0.20399999999999999</v>
       </c>
       <c r="E94">
-        <v>0.15</v>
+        <v>0.109</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.15">
@@ -16868,16 +16843,16 @@
         <v>940000</v>
       </c>
       <c r="B95">
-        <v>0.41</v>
+        <v>0.39500000000000002</v>
       </c>
       <c r="C95">
-        <v>0.16</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="D95">
-        <v>0.23</v>
+        <v>0.20899999999999999</v>
       </c>
       <c r="E95">
-        <v>0.11</v>
+        <v>0.113</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.15">
@@ -16885,16 +16860,16 @@
         <v>950000</v>
       </c>
       <c r="B96">
-        <v>0.39</v>
+        <v>0.42</v>
       </c>
       <c r="C96">
-        <v>0.16</v>
+        <v>0.14299999999999999</v>
       </c>
       <c r="D96">
-        <v>0.2</v>
+        <v>0.215</v>
       </c>
       <c r="E96">
-        <v>0.1</v>
+        <v>0.11799999999999999</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.15">
@@ -16902,16 +16877,16 @@
         <v>960000</v>
       </c>
       <c r="B97">
-        <v>0.4</v>
+        <v>0.41699999999999998</v>
       </c>
       <c r="C97">
-        <v>0.14000000000000001</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="D97">
-        <v>0.23</v>
+        <v>0.21199999999999999</v>
       </c>
       <c r="E97">
-        <v>0.15</v>
+        <v>0.123</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.15">
@@ -16919,16 +16894,16 @@
         <v>970000</v>
       </c>
       <c r="B98">
-        <v>0.41</v>
+        <v>0.41499999999999998</v>
       </c>
       <c r="C98">
-        <v>0.16</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="D98">
-        <v>0.22</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="E98">
-        <v>0.13</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.15">
@@ -16936,16 +16911,16 @@
         <v>980000</v>
       </c>
       <c r="B99">
-        <v>0.4</v>
+        <v>0.42199999999999999</v>
       </c>
       <c r="C99">
-        <v>0.16</v>
+        <v>0.153</v>
       </c>
       <c r="D99">
-        <v>0.25</v>
+        <v>0.22800000000000001</v>
       </c>
       <c r="E99">
-        <v>0.16</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.15">
@@ -16953,33 +16928,16 @@
         <v>990000</v>
       </c>
       <c r="B100">
-        <v>0.39</v>
+        <v>0.42799999999999999</v>
       </c>
       <c r="C100">
-        <v>0.15</v>
+        <v>0.156</v>
       </c>
       <c r="D100">
-        <v>0.22</v>
+        <v>0.224</v>
       </c>
       <c r="E100">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A101">
-        <v>1000000</v>
-      </c>
-      <c r="B101">
-        <v>0.39</v>
-      </c>
-      <c r="C101">
-        <v>0.16</v>
-      </c>
-      <c r="D101">
-        <v>0.23</v>
-      </c>
-      <c r="E101">
-        <v>0.13</v>
+        <v>0.121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>